<commit_message>
BOM updates -- cost of manufacturing
</commit_message>
<xml_diff>
--- a/documentation/BOM_3d-viz-rig.xlsx
+++ b/documentation/BOM_3d-viz-rig.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="120">
   <si>
     <t>System</t>
   </si>
@@ -367,6 +367,18 @@
   </si>
   <si>
     <t>https://www.bhphotovideo.com/bnh/controller/home?O=invoice&amp;A=details&amp;Q=&amp;sku=1030864&amp;is=REG&amp;mode=edu</t>
+  </si>
+  <si>
+    <t>https://github.com/UCSD-E4E/3d-visualization-system/blob/master/CAD/Base%20plate.SLDPRT</t>
+  </si>
+  <si>
+    <t>https://github.com/UCSD-E4E/3d-visualization-system/blob/master/CAD/enclosure%20tube%20holder.SLDPRT</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>(included in machining cost)</t>
   </si>
 </sst>
 </file>
@@ -797,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -815,7 +827,7 @@
     <col min="9" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -840,8 +852,11 @@
       <c r="H1" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -868,7 +883,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
@@ -892,7 +907,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
@@ -916,7 +931,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="B5" s="3" t="s">
         <v>32</v>
       </c>
@@ -940,7 +955,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
@@ -961,7 +976,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
@@ -985,7 +1000,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1006,7 +1021,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
@@ -1027,7 +1042,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
@@ -1048,7 +1063,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
@@ -1072,7 +1087,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="B12" s="3" t="s">
         <v>95</v>
       </c>
@@ -1096,7 +1111,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -1109,8 +1124,21 @@
       <c r="D15" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="E15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
+      <c r="G15" s="12">
+        <v>175</v>
+      </c>
+      <c r="H15" s="12">
+        <f>F15*G15</f>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="B16" s="3" t="s">
         <v>59</v>
       </c>
@@ -1120,8 +1148,21 @@
       <c r="D16" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="E16" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" s="6">
+        <v>4</v>
+      </c>
+      <c r="G16" s="12">
+        <v>125</v>
+      </c>
+      <c r="H16" s="12">
+        <f>F16*G16</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="B17" s="3" t="s">
         <v>43</v>
       </c>
@@ -1131,8 +1172,11 @@
       <c r="D17" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="B18" s="3" t="s">
         <v>97</v>
       </c>
@@ -1142,8 +1186,11 @@
       <c r="D18" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="B19" s="3" t="s">
         <v>52</v>
       </c>
@@ -1167,7 +1214,7 @@
         <v>64.95</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="B20" s="3" t="s">
         <v>54</v>
       </c>
@@ -1191,7 +1238,7 @@
         <v>64.95</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:9">
       <c r="B21" s="3" t="s">
         <v>113</v>
       </c>
@@ -1215,7 +1262,7 @@
         <v>99.9</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="B22" s="3" t="s">
         <v>80</v>
       </c>
@@ -1239,7 +1286,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9">
       <c r="B23" s="3" t="s">
         <v>85</v>
       </c>
@@ -1263,7 +1310,7 @@
         <v>3.06</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9">
       <c r="B24" s="3" t="s">
         <v>108</v>
       </c>
@@ -1287,7 +1334,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:9">
       <c r="B25" s="3" t="s">
         <v>111</v>
       </c>
@@ -1311,7 +1358,7 @@
         <v>31.52</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
         <v>76</v>
       </c>
@@ -1338,7 +1385,7 @@
         <v>999.98</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9">
       <c r="B28" s="3" t="s">
         <v>41</v>
       </c>
@@ -1359,7 +1406,7 @@
         <v>699.98</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:9">
       <c r="B29" s="3" t="s">
         <v>66</v>
       </c>
@@ -1367,7 +1414,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="B30" t="s">
         <v>88</v>
       </c>
@@ -1391,7 +1438,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:9">
       <c r="B31" s="3" t="s">
         <v>77</v>
       </c>
@@ -1619,7 +1666,7 @@
       </c>
       <c r="H46" s="12">
         <f>SUM(H2:H43)</f>
-        <v>5334.14</v>
+        <v>6009.1400000000012</v>
       </c>
     </row>
   </sheetData>
@@ -1651,6 +1698,8 @@
     <hyperlink ref="E24" r:id="rId25" location="92196A148" tooltip="Close"/>
     <hyperlink ref="E25" r:id="rId26"/>
     <hyperlink ref="E21" r:id="rId27"/>
+    <hyperlink ref="E15" r:id="rId28"/>
+    <hyperlink ref="E16" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>